<commit_message>
reporte para defecto PE-44
</commit_message>
<xml_diff>
--- a/tests_cases/PE44 - TC -04.xlsx
+++ b/tests_cases/PE44 - TC -04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Q-CHECK\tests_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3E67F0-A5BA-411E-B103-700523A8A331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573F3097-46DC-43C8-A70E-D3D17D52011F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
   </bookViews>
   <sheets>
     <sheet name="TC - Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -102,73 +102,36 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Search bar: Server error displayed when user users the search functionality</t>
-  </si>
-  <si>
     <t>Description / Overview</t>
   </si>
   <si>
-    <t>Typing any text on the search bar redirects user to an error page</t>
-  </si>
-  <si>
     <t>Reproduction Steps</t>
   </si>
   <si>
-    <t xml:space="preserve">1- Open the application page https://demo.opencart.com/ </t>
-  </si>
-  <si>
-    <t>2- Type "example" on the search bar</t>
-  </si>
-  <si>
-    <t>3- Click the "Search" button</t>
-  </si>
-  <si>
     <t>Expected Behavior</t>
   </si>
   <si>
-    <t>A page showing the search results is displayed</t>
-  </si>
-  <si>
     <t>Actual Behavior</t>
   </si>
   <si>
-    <t>The Page shows an error page with the text "Internal Server Error!"</t>
-  </si>
-  <si>
     <t>Incidence / Severity / Probability of reproduction</t>
   </si>
   <si>
-    <t>Critical severity - The search functionality does not work</t>
-  </si>
-  <si>
     <t>100% reproduction rate</t>
   </si>
   <si>
     <t>Story and Acceptance Criteria affected</t>
   </si>
   <si>
-    <t>Affected User Story: US-18</t>
-  </si>
-  <si>
     <t>Browsers tested</t>
   </si>
   <si>
-    <t>Google Chrome, v107</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
-    <t xml:space="preserve">QA environment, https://demo.opencart.com/ </t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>- The search request returns a 302 (redirection) code, so the error might be caused by an incorrect configuration setting.
-- Test Case TC-013 covers this scenario</t>
-  </si>
-  <si>
     <t>David Monsalve</t>
   </si>
   <si>
@@ -269,13 +232,58 @@
   </si>
   <si>
     <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>Check-Out: No funciona.</t>
+  </si>
+  <si>
+    <t>Cuando el usuario procede a pagar los productos del carrito, el boton de check-out no nos lleva a la pagina de pago.</t>
+  </si>
+  <si>
+    <t>1 - Ir al ecommerce.</t>
+  </si>
+  <si>
+    <t>2 - Registrarse o iniciar sesion.</t>
+  </si>
+  <si>
+    <t>4 - Click al boton de añadir al carrito.</t>
+  </si>
+  <si>
+    <t>3- Escoger un producto (Escoger uno directamente desde el landing page para mas facilidad).</t>
+  </si>
+  <si>
+    <t>Carga la pagina de pago.</t>
+  </si>
+  <si>
+    <t>5 -  Click al boton del carrito. (en nav-bar )</t>
+  </si>
+  <si>
+    <t>5 -  Click al boton de "proceed checkout."</t>
+  </si>
+  <si>
+    <t>Nos dice que la pagina no existe.</t>
+  </si>
+  <si>
+    <t>Crítico. Los usuarios no pueden comprarnos nada.</t>
+  </si>
+  <si>
+    <t>PE-44.</t>
+  </si>
+  <si>
+    <t>QA environment, http://127.0.0.1:5000/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puede ser que el documento "check-out.html" (por llamar de una forma a la pagina de pago) no esté ubicado en el lugar que deberia, haciendose imposible de encontrar por nuestro navegador. </t>
+  </si>
+  <si>
+    <t>Brave, V 1.45.131</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,23 +309,8 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -412,6 +405,36 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -890,293 +913,297 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1207,22 +1234,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>35719</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>55562</xdr:rowOff>
+      <xdr:colOff>142645</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1608625</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1580753</xdr:rowOff>
+      <xdr:colOff>7364015</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>3452812</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF530E03-E415-4115-91D9-304ABFC4F373}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D969D56A-B38F-A535-DE1D-7E32AF2B06FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1238,8 +1265,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2266157" y="2063750"/>
-          <a:ext cx="1572906" cy="1525191"/>
+          <a:off x="2267911" y="3036094"/>
+          <a:ext cx="7221370" cy="3417093"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1550,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3CCAC7-6C0E-44CD-ADA1-CF7A0722318C}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1573,523 +1600,523 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="83"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="85"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="86">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="87"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="15">
+        <v>2</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="91"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="73"/>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="89"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="77"/>
+      <c r="D14" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="79"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="81"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="70"/>
+      <c r="D16" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="72"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40">
+        <v>1</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="60"/>
+      <c r="D17" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="61"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="41">
+        <v>2</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="60"/>
+      <c r="D18" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="60"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="51"/>
+    </row>
+    <row r="19" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41">
+        <v>2</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="60"/>
+      <c r="D19" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="60"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="40">
+        <v>3</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="60"/>
+      <c r="D20" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="61"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="41">
+        <v>4</v>
+      </c>
+      <c r="B21" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="60"/>
+      <c r="D21" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="64"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="42">
+        <v>5</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="66"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="49">
+        <v>6</v>
+      </c>
+      <c r="B23" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="67"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="50">
+        <v>7</v>
+      </c>
+      <c r="B24" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="68"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="57"/>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-    </row>
-    <row r="2" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="64">
-        <v>0.1</v>
-      </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="102" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="25"/>
-    </row>
-    <row r="6" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="26">
-        <v>1</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="26">
-        <v>2</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="19"/>
-    </row>
-    <row r="10" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="19"/>
-    </row>
-    <row r="11" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19"/>
-    </row>
-    <row r="12" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="72"/>
-      <c r="I12" s="19"/>
-    </row>
-    <row r="13" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="19"/>
-    </row>
-    <row r="14" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="78"/>
-      <c r="I14" s="19"/>
-    </row>
-    <row r="15" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="80"/>
-      <c r="I15" s="19"/>
-    </row>
-    <row r="16" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="82"/>
-      <c r="D16" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="84"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="19"/>
-    </row>
-    <row r="17" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51">
-        <v>1</v>
-      </c>
-      <c r="B17" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="87"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17" s="19"/>
-    </row>
-    <row r="18" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52">
-        <v>2</v>
-      </c>
-      <c r="B18" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="86"/>
-      <c r="D18" s="88" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="100"/>
-    </row>
-    <row r="19" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
-        <v>2</v>
-      </c>
-      <c r="B19" s="88" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="88" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" s="19"/>
-    </row>
-    <row r="20" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51">
-        <v>3</v>
-      </c>
-      <c r="B20" s="85" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="86"/>
-      <c r="D20" s="87" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="87"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" s="19"/>
-    </row>
-    <row r="21" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52">
-        <v>4</v>
-      </c>
-      <c r="B21" s="88" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="86"/>
-      <c r="D21" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="71"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" s="19"/>
-    </row>
-    <row r="22" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53">
-        <v>5</v>
-      </c>
-      <c r="B22" s="70" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="90" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="91"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="19"/>
-    </row>
-    <row r="23" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="98">
-        <v>6</v>
-      </c>
-      <c r="B23" s="96" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="96"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" s="19"/>
-    </row>
-    <row r="24" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="99">
-        <v>7</v>
-      </c>
-      <c r="B24" s="97" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="97"/>
-      <c r="D24" s="97" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="97"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="I24" s="19"/>
-    </row>
-    <row r="25" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="92"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="19"/>
-    </row>
-    <row r="26" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="92"/>
-      <c r="C26" s="92"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="95"/>
-      <c r="I26" s="19"/>
-    </row>
-    <row r="27" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="92"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="94" t="s">
-        <v>75</v>
-      </c>
-      <c r="H27" s="94"/>
-      <c r="I27" s="19"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="92"/>
-      <c r="C28" s="92"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="93"/>
-      <c r="H28" s="93"/>
-      <c r="I28" s="19"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="92"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="93"/>
-      <c r="I29" s="19"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="92"/>
-      <c r="C30" s="92"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="19"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="8"/>
     </row>
     <row r="31" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="89"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="8"/>
     </row>
     <row r="32" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
     </row>
     <row r="37" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
@@ -2102,23 +2129,24 @@
     <row r="65" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:E20"/>
@@ -2131,24 +2159,23 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2157,115 +2184,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19C3A39-FFB1-416B-9AA1-6DCAB5934A9A}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="63.7109375" customWidth="1"/>
+    <col min="2" max="2" width="111.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="103" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="92"/>
+    </row>
+    <row r="3" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="93" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="104" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="92"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="97" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="98" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="99" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="99" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="99" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="99" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="95" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B11" s="100" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B13" s="100" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="279.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="94" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="B15" s="97" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="96"/>
+      <c r="B16" s="99" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="95" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="B18" s="101" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B20" s="100" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="95" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="B22" s="100" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>42</v>
+      <c r="B24" s="102" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2276,21 +2325,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005ACBF82FF32280448C88565210D23A47" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="97d18655ea211e7533acd5a2318ca8a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c71177d-84a1-4dd9-b712-f5a48054c455" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4416c93f0313e0694190cc26fdb99745" ns2:_="">
     <xsd:import namespace="9c71177d-84a1-4dd9-b712-f5a48054c455"/>
@@ -2422,24 +2456,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D9EE348-9CCE-471E-BE4A-E92394DC64F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E2D575-FFD0-4884-BFC5-ACB7CFB69618}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69FDEB6B-1403-4F25-B1A4-5EE5DE15C544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2455,4 +2487,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E2D575-FFD0-4884-BFC5-ACB7CFB69618}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D9EE348-9CCE-471E-BE4A-E92394DC64F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>